<commit_message>
New prompt, some prints and conditional pairwise start
</commit_message>
<xml_diff>
--- a/runs_summary.xlsx
+++ b/runs_summary.xlsx
@@ -425,7 +425,7 @@
     <outlinePr summaryBelow="1" summaryRight="1"/>
     <pageSetUpPr/>
   </sheetPr>
-  <dimension ref="A1:Y30"/>
+  <dimension ref="A1:Y34"/>
   <sheetViews>
     <sheetView workbookViewId="0">
       <selection activeCell="A1" sqref="A1"/>
@@ -3257,6 +3257,378 @@
         <v>2935</v>
       </c>
     </row>
+    <row r="31">
+      <c r="A31" t="inlineStr">
+        <is>
+          <t>run_2025-09-29T21-42-48.129862p00-00_96d301d8.json</t>
+        </is>
+      </c>
+      <c r="B31" t="inlineStr">
+        <is>
+          <t>96d301d8</t>
+        </is>
+      </c>
+      <c r="C31" t="inlineStr">
+        <is>
+          <t>success</t>
+        </is>
+      </c>
+      <c r="D31" t="inlineStr">
+        <is>
+          <t>2025-09-29T21-42-48.129862p00-00</t>
+        </is>
+      </c>
+      <c r="E31" t="n">
+        <v>1</v>
+      </c>
+      <c r="F31" t="inlineStr">
+        <is>
+          <t>test</t>
+        </is>
+      </c>
+      <c r="G31" t="inlineStr">
+        <is>
+          <t>openai/gpt-5-mini</t>
+        </is>
+      </c>
+      <c r="H31" t="inlineStr">
+        <is>
+          <t>realpariwise-alltools-gpt5mini-1-test</t>
+        </is>
+      </c>
+      <c r="I31" t="inlineStr">
+        <is>
+          <t>coherence_check, counterfactual_pairs</t>
+        </is>
+      </c>
+      <c r="J31" t="n">
+        <v>0.6666666666666666</v>
+      </c>
+      <c r="K31" t="n">
+        <v>0.3333333333333333</v>
+      </c>
+      <c r="L31" t="n">
+        <v>0.4444444444444444</v>
+      </c>
+      <c r="M31" t="n">
+        <v>0</v>
+      </c>
+      <c r="N31" t="n">
+        <v>1</v>
+      </c>
+      <c r="O31" t="n">
+        <v>0.3333333333333333</v>
+      </c>
+      <c r="P31" t="n">
+        <v>0.5</v>
+      </c>
+      <c r="Q31" t="n">
+        <v>3</v>
+      </c>
+      <c r="R31" t="n">
+        <v>0.5</v>
+      </c>
+      <c r="S31" t="n">
+        <v>0.3333333333333333</v>
+      </c>
+      <c r="T31" t="n">
+        <v>0.4</v>
+      </c>
+      <c r="U31" t="n">
+        <v>3</v>
+      </c>
+      <c r="V31" t="n">
+        <v>0.9166666666666666</v>
+      </c>
+      <c r="W31" t="n">
+        <v>0.9777777777777777</v>
+      </c>
+      <c r="X31" t="n">
+        <v>0.946236559139785</v>
+      </c>
+      <c r="Y31" t="n">
+        <v>45</v>
+      </c>
+    </row>
+    <row r="32">
+      <c r="A32" t="inlineStr">
+        <is>
+          <t>run_2025-09-29T22-42-49.468928p00-00_fc95b218.json</t>
+        </is>
+      </c>
+      <c r="B32" t="inlineStr">
+        <is>
+          <t>fc95b218</t>
+        </is>
+      </c>
+      <c r="C32" t="inlineStr">
+        <is>
+          <t>success</t>
+        </is>
+      </c>
+      <c r="D32" t="inlineStr">
+        <is>
+          <t>2025-09-29T22-42-49.468928p00-00</t>
+        </is>
+      </c>
+      <c r="E32" t="n">
+        <v>1</v>
+      </c>
+      <c r="F32" t="inlineStr">
+        <is>
+          <t>test</t>
+        </is>
+      </c>
+      <c r="G32" t="inlineStr">
+        <is>
+          <t>openai/gpt-5-mini</t>
+        </is>
+      </c>
+      <c r="H32" t="inlineStr">
+        <is>
+          <t>realpariwise-alltools-gpt5mini-1-test</t>
+        </is>
+      </c>
+      <c r="I32" t="inlineStr">
+        <is>
+          <t>coherence_check, counterfactual_pairs</t>
+        </is>
+      </c>
+      <c r="J32" t="n">
+        <v>0</v>
+      </c>
+      <c r="K32" t="n">
+        <v>0</v>
+      </c>
+      <c r="L32" t="n">
+        <v>0</v>
+      </c>
+      <c r="M32" t="n">
+        <v>0</v>
+      </c>
+      <c r="N32" t="n">
+        <v>0</v>
+      </c>
+      <c r="O32" t="n">
+        <v>0</v>
+      </c>
+      <c r="P32" t="n">
+        <v>0</v>
+      </c>
+      <c r="Q32" t="n">
+        <v>3</v>
+      </c>
+      <c r="R32" t="n">
+        <v>0</v>
+      </c>
+      <c r="S32" t="n">
+        <v>0</v>
+      </c>
+      <c r="T32" t="n">
+        <v>0</v>
+      </c>
+      <c r="U32" t="n">
+        <v>3</v>
+      </c>
+      <c r="V32" t="n">
+        <v>0.8823529411764706</v>
+      </c>
+      <c r="W32" t="n">
+        <v>1</v>
+      </c>
+      <c r="X32" t="n">
+        <v>0.9375</v>
+      </c>
+      <c r="Y32" t="n">
+        <v>45</v>
+      </c>
+    </row>
+    <row r="33">
+      <c r="A33" t="inlineStr">
+        <is>
+          <t>run_2025-09-29T22-50-16.237030p00-00_7d12cbea.json</t>
+        </is>
+      </c>
+      <c r="B33" t="inlineStr">
+        <is>
+          <t>7d12cbea</t>
+        </is>
+      </c>
+      <c r="C33" t="inlineStr">
+        <is>
+          <t>success</t>
+        </is>
+      </c>
+      <c r="D33" t="inlineStr">
+        <is>
+          <t>2025-09-29T22-50-16.237030p00-00</t>
+        </is>
+      </c>
+      <c r="E33" t="n">
+        <v>1</v>
+      </c>
+      <c r="F33" t="inlineStr">
+        <is>
+          <t>test</t>
+        </is>
+      </c>
+      <c r="G33" t="inlineStr">
+        <is>
+          <t>openai/gpt-5-mini</t>
+        </is>
+      </c>
+      <c r="H33" t="inlineStr">
+        <is>
+          <t>realpariwise-alltools-gpt5mini-1-test</t>
+        </is>
+      </c>
+      <c r="I33" t="inlineStr">
+        <is>
+          <t>coherence_check, counterfactual_pairs</t>
+        </is>
+      </c>
+      <c r="J33" t="n">
+        <v>0.6666666666666666</v>
+      </c>
+      <c r="K33" t="n">
+        <v>0.3333333333333333</v>
+      </c>
+      <c r="L33" t="n">
+        <v>0.4444444444444444</v>
+      </c>
+      <c r="M33" t="n">
+        <v>0</v>
+      </c>
+      <c r="N33" t="n">
+        <v>1</v>
+      </c>
+      <c r="O33" t="n">
+        <v>0.3333333333333333</v>
+      </c>
+      <c r="P33" t="n">
+        <v>0.5</v>
+      </c>
+      <c r="Q33" t="n">
+        <v>3</v>
+      </c>
+      <c r="R33" t="n">
+        <v>0.5</v>
+      </c>
+      <c r="S33" t="n">
+        <v>0.3333333333333333</v>
+      </c>
+      <c r="T33" t="n">
+        <v>0.4</v>
+      </c>
+      <c r="U33" t="n">
+        <v>3</v>
+      </c>
+      <c r="V33" t="n">
+        <v>0.9166666666666666</v>
+      </c>
+      <c r="W33" t="n">
+        <v>0.9777777777777777</v>
+      </c>
+      <c r="X33" t="n">
+        <v>0.946236559139785</v>
+      </c>
+      <c r="Y33" t="n">
+        <v>45</v>
+      </c>
+    </row>
+    <row r="34">
+      <c r="A34" t="inlineStr">
+        <is>
+          <t>run_2025-09-30T00-31-31.473510p00-00_4bfc73d7.json</t>
+        </is>
+      </c>
+      <c r="B34" t="inlineStr">
+        <is>
+          <t>4bfc73d7</t>
+        </is>
+      </c>
+      <c r="C34" t="inlineStr">
+        <is>
+          <t>success</t>
+        </is>
+      </c>
+      <c r="D34" t="inlineStr">
+        <is>
+          <t>2025-09-30T00-31-31.473510p00-00</t>
+        </is>
+      </c>
+      <c r="E34" t="n">
+        <v>50</v>
+      </c>
+      <c r="F34" t="inlineStr">
+        <is>
+          <t>test</t>
+        </is>
+      </c>
+      <c r="G34" t="inlineStr">
+        <is>
+          <t>openai/gpt-5-mini</t>
+        </is>
+      </c>
+      <c r="H34" t="inlineStr">
+        <is>
+          <t>realpariwise-alltools-gpt5mini-50-test</t>
+        </is>
+      </c>
+      <c r="I34" t="inlineStr">
+        <is>
+          <t>coherence_check, counterfactual_pairs</t>
+        </is>
+      </c>
+      <c r="J34" t="n">
+        <v>0.3872549019607843</v>
+      </c>
+      <c r="K34" t="n">
+        <v>0.6171875</v>
+      </c>
+      <c r="L34" t="n">
+        <v>0.4759036144578314</v>
+      </c>
+      <c r="M34" t="n">
+        <v>1</v>
+      </c>
+      <c r="N34" t="n">
+        <v>0.3674418604651163</v>
+      </c>
+      <c r="O34" t="n">
+        <v>0.6171875</v>
+      </c>
+      <c r="P34" t="n">
+        <v>0.4606413994169096</v>
+      </c>
+      <c r="Q34" t="n">
+        <v>128</v>
+      </c>
+      <c r="R34" t="n">
+        <v>0.4093264248704663</v>
+      </c>
+      <c r="S34" t="n">
+        <v>0.6171875</v>
+      </c>
+      <c r="T34" t="n">
+        <v>0.4922118380062304</v>
+      </c>
+      <c r="U34" t="n">
+        <v>128</v>
+      </c>
+      <c r="V34" t="n">
+        <v>0.9698167445203019</v>
+      </c>
+      <c r="W34" t="n">
+        <v>0.9195911413969335</v>
+      </c>
+      <c r="X34" t="n">
+        <v>0.9440363763553691</v>
+      </c>
+      <c r="Y34" t="n">
+        <v>2935</v>
+      </c>
+    </row>
   </sheetData>
   <pageMargins left="0.75" right="0.75" top="1" bottom="1" header="0.5" footer="0.5"/>
 </worksheet>

</xml_diff>